<commit_message>
finding the medium of models
</commit_message>
<xml_diff>
--- a/Metabolic Models (mixed culture)/Kinetic model MCF v4 (updated)/myMCFModelStructure.xlsx
+++ b/Metabolic Models (mixed culture)/Kinetic model MCF v4 (updated)/myMCFModelStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/lucas_vanderhauwaert_usc_es/Documents/Alquimia/Model_Mateo/Kinetic model MCF v4 (updated)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\PycharmProjects\Alquimia\Metabolic Models (mixed culture)\Kinetic model MCF v4 (updated)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="665" documentId="109_{2AED3B22-32A6-484E-AB35-4CDA822F70E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19BF7908-9A35-44E4-A458-177F3C223E72}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D79255A-6737-453E-842C-6C337C3A1111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{FB00034E-A85C-4875-A89F-141F6387C86F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FB00034E-A85C-4875-A89F-141F6387C86F}"/>
   </bookViews>
   <sheets>
     <sheet name="Compounds" sheetId="2" r:id="rId1"/>
@@ -1613,7 +1613,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1630,458 +1630,22 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A687BD58-8BA3-41E8-B964-DF2E4C6C25D2}"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2150,9 +1714,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2190,7 +1754,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2296,7 +1860,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2438,7 +2002,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2462,13 +2026,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBEAA9A-39F9-4588-9ED7-2006711C63B8}">
   <dimension ref="B2:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
@@ -3358,7 +2924,7 @@
       <c r="D32">
         <v>30</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="15">
         <v>0</v>
       </c>
       <c r="F32" s="11">
@@ -3416,7 +2982,7 @@
       <c r="D34">
         <v>32</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="15">
         <v>0</v>
       </c>
       <c r="F34" s="11">
@@ -3444,10 +3010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDCF2C4-CE67-4FC6-A97F-9A96EFF9F364}">
-  <dimension ref="A2:AH51"/>
+  <dimension ref="B2:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3461,7 +3027,7 @@
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>446</v>
       </c>
@@ -3483,13 +3049,13 @@
       <c r="J2" t="s">
         <v>431</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" t="s">
         <v>437</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" t="s">
         <v>438</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" t="s">
         <v>439</v>
       </c>
       <c r="N2" t="s">
@@ -3516,18 +3082,17 @@
       <c r="U2" s="10"/>
       <c r="Y2" s="9"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>276</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3">
         <v>3</v>
       </c>
       <c r="G3">
@@ -3542,13 +3107,13 @@
       <c r="J3">
         <v>7</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3">
         <v>8</v>
       </c>
-      <c r="L3" s="21">
+      <c r="L3">
         <v>9</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3">
         <v>10</v>
       </c>
       <c r="N3">
@@ -3573,8 +3138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A4" s="26"/>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>433</v>
       </c>
@@ -3584,10 +3148,10 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="21">
-        <v>0</v>
-      </c>
-      <c r="F4" s="21">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
@@ -3602,13 +3166,13 @@
       <c r="J4">
         <v>0.26</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4">
         <v>0.65</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4">
         <v>0.65</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4">
         <v>0.65</v>
       </c>
       <c r="N4">
@@ -3623,7 +3187,7 @@
       <c r="Q4">
         <v>1</v>
       </c>
-      <c r="R4" s="20">
+      <c r="R4" s="9">
         <f>1-R6</f>
         <v>0.94573643410852715</v>
       </c>
@@ -3634,8 +3198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A5" s="26"/>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>434</v>
       </c>
@@ -3645,10 +3208,10 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="21">
-        <v>0</v>
-      </c>
-      <c r="F5" s="21">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
@@ -3663,13 +3226,13 @@
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5" s="21">
-        <v>0</v>
-      </c>
-      <c r="L5" s="21">
-        <v>0</v>
-      </c>
-      <c r="M5" s="21">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
@@ -3694,8 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A6" s="26"/>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>435</v>
       </c>
@@ -3705,10 +3267,10 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
@@ -3723,13 +3285,13 @@
       <c r="J6">
         <v>0.74</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6">
         <v>0.35</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6">
         <v>0.35</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6">
         <v>0.35</v>
       </c>
       <c r="N6">
@@ -3741,10 +3303,10 @@
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6" s="21">
-        <v>0</v>
-      </c>
-      <c r="R6" s="20">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6" s="9">
         <v>5.4263565891472867E-2</v>
       </c>
       <c r="S6">
@@ -3754,345 +3316,336 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A7" s="26"/>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>427</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
-      <c r="D7" s="17">
-        <v>0</v>
-      </c>
-      <c r="E7" s="17">
-        <v>0</v>
-      </c>
-      <c r="F7" s="17">
-        <v>0</v>
-      </c>
-      <c r="G7" s="17">
+      <c r="D7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
         <v>0.26807794200202667</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="16">
         <v>0.69671550043847885</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="16">
         <v>0.66170923646479518</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="16">
         <v>0</v>
       </c>
       <c r="K7" s="12">
         <v>0.48668243264812233</v>
       </c>
-      <c r="L7" s="20">
+      <c r="L7" s="9">
         <v>0.42563574974946605</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="9">
         <v>0.55527557299379682</v>
       </c>
-      <c r="N7" s="20">
+      <c r="N7" s="9">
         <v>0.8270061226729557</v>
       </c>
-      <c r="O7" s="20">
+      <c r="O7" s="9">
         <v>0.79124534651786504</v>
       </c>
-      <c r="P7" s="20">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="20">
+      <c r="P7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="9">
         <v>0.12312188443972553</v>
       </c>
-      <c r="R7" s="20">
+      <c r="R7" s="9">
         <v>0.29140826873385017</v>
       </c>
-      <c r="S7" s="17">
+      <c r="S7" s="16">
         <v>5.7568635649161828E-2</v>
       </c>
-      <c r="T7" s="17">
+      <c r="T7" s="16">
         <v>0.77564153479220055</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A8" s="26"/>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>419</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>1</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>1</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>1</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="16">
         <v>0.18185111132644197</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <v>9.6970114024897247E-2</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <v>9.2935787634504732E-2</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="16">
         <v>0.92464927100560868</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="9">
         <v>0.25736882655313603</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="9">
         <v>0.18855185625605825</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="9">
         <v>0.26836735525141636</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="9">
         <v>3.3458278923208622E-2</v>
       </c>
-      <c r="O8" s="20">
+      <c r="O8" s="9">
         <v>1.4839425586983753E-2</v>
       </c>
-      <c r="P8" s="20">
+      <c r="P8" s="9">
         <v>0.63070714691274665</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="9">
         <v>0.19597168521154626</v>
       </c>
-      <c r="R8" s="20">
+      <c r="R8" s="9">
         <v>0.28578811369509044</v>
       </c>
-      <c r="S8" s="17">
+      <c r="S8" s="16">
         <v>6.8399077111503642E-2</v>
       </c>
-      <c r="T8" s="17">
+      <c r="T8" s="16">
         <v>0.1481389218545652</v>
       </c>
-      <c r="U8" s="21"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A9" s="26"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>420</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
-      <c r="D9" s="17">
-        <v>0</v>
-      </c>
-      <c r="E9" s="17">
-        <v>0</v>
-      </c>
-      <c r="F9" s="17">
-        <v>0</v>
-      </c>
-      <c r="G9" s="17">
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
         <v>0.41328682725312443</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="16">
         <v>5.3879332033909044E-2</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="16">
         <v>0.17796472422695028</v>
       </c>
-      <c r="J9" s="17">
-        <v>0</v>
-      </c>
-      <c r="K9" s="20">
+      <c r="J9" s="16">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9">
         <v>0.21900709469165502</v>
       </c>
-      <c r="L9" s="20">
+      <c r="L9" s="9">
         <v>0.10640893743736646</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="9">
         <v>0.1388188932484492</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="9">
         <v>0.10644633262127154</v>
       </c>
-      <c r="O9" s="20">
+      <c r="O9" s="9">
         <v>0.17052701433574677</v>
       </c>
-      <c r="P9" s="20">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="20">
-        <v>0</v>
-      </c>
-      <c r="R9" s="20">
+      <c r="P9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>0</v>
+      </c>
+      <c r="R9" s="9">
         <v>0.15691214470284237</v>
       </c>
-      <c r="S9" s="17">
+      <c r="S9" s="16">
         <v>0.84074194979296779</v>
       </c>
-      <c r="T9" s="17">
+      <c r="T9" s="16">
         <v>2.2098049424279214E-2</v>
       </c>
-      <c r="U9" s="21"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>421</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
-      <c r="D10" s="17">
-        <v>0</v>
-      </c>
-      <c r="E10" s="17">
-        <v>0</v>
-      </c>
-      <c r="F10" s="17">
-        <v>0</v>
-      </c>
-      <c r="G10" s="17">
+      <c r="D10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
         <v>0.13678411941840696</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="16">
         <v>0.15243505350271491</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="16">
         <v>6.7390251673749832E-2</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="16">
         <v>7.5350728994391339E-2</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="9">
         <v>3.6941646107086806E-2</v>
       </c>
-      <c r="L10" s="20">
+      <c r="L10" s="9">
         <v>0.27940345655710913</v>
       </c>
-      <c r="M10" s="20">
+      <c r="M10" s="9">
         <v>3.7538178506337602E-2</v>
       </c>
-      <c r="N10" s="20">
+      <c r="N10" s="9">
         <v>3.3089265782564103E-2</v>
       </c>
-      <c r="O10" s="20">
+      <c r="O10" s="9">
         <v>2.3388213559404462E-2</v>
       </c>
-      <c r="P10" s="20">
+      <c r="P10" s="9">
         <v>0.36929285308725329</v>
       </c>
-      <c r="Q10" s="20">
+      <c r="Q10" s="9">
         <v>0.68090643034872822</v>
       </c>
-      <c r="R10" s="20">
+      <c r="R10" s="9">
         <v>0.18519379844961248</v>
       </c>
-      <c r="S10" s="17">
+      <c r="S10" s="16">
         <v>3.3290337446366773E-2</v>
       </c>
-      <c r="T10" s="17">
+      <c r="T10" s="16">
         <v>5.4121493928955031E-2</v>
       </c>
-      <c r="U10" s="21"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A11" s="26"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>422</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
-      <c r="D11" s="17">
-        <v>0</v>
-      </c>
-      <c r="E11" s="17">
-        <v>0</v>
-      </c>
-      <c r="F11" s="17">
-        <v>0</v>
-      </c>
-      <c r="G11" s="17">
-        <v>0</v>
-      </c>
-      <c r="H11" s="17">
-        <v>0</v>
-      </c>
-      <c r="I11" s="17">
-        <v>0</v>
-      </c>
-      <c r="J11" s="17">
-        <v>0</v>
-      </c>
-      <c r="K11" s="20">
-        <v>0</v>
-      </c>
-      <c r="L11" s="20">
-        <v>0</v>
-      </c>
-      <c r="M11" s="20">
-        <v>0</v>
-      </c>
-      <c r="N11" s="20">
-        <v>0</v>
-      </c>
-      <c r="O11" s="20">
-        <v>0</v>
-      </c>
-      <c r="P11" s="20">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="20">
-        <v>0</v>
-      </c>
-      <c r="R11" s="20">
-        <v>0</v>
-      </c>
-      <c r="S11" s="17">
-        <v>0</v>
-      </c>
-      <c r="T11" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A12" s="26"/>
+      <c r="D11" s="16">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0</v>
+      </c>
+      <c r="P11" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>0</v>
+      </c>
+      <c r="R11" s="9">
+        <v>0</v>
+      </c>
+      <c r="S11" s="16">
+        <v>0</v>
+      </c>
+      <c r="T11" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>423</v>
       </c>
       <c r="C12">
         <v>9</v>
       </c>
-      <c r="D12" s="17">
-        <v>0</v>
-      </c>
-      <c r="E12" s="17">
-        <v>0</v>
-      </c>
-      <c r="F12" s="17">
-        <v>0</v>
-      </c>
-      <c r="G12" s="17">
-        <v>0</v>
-      </c>
-      <c r="H12" s="17">
-        <v>0</v>
-      </c>
-      <c r="I12" s="17">
-        <v>0</v>
-      </c>
-      <c r="J12" s="17">
-        <v>0</v>
-      </c>
-      <c r="K12" s="20">
-        <v>0</v>
-      </c>
-      <c r="L12" s="20">
-        <v>0</v>
-      </c>
-      <c r="M12" s="20">
+      <c r="D12" s="16">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0</v>
+      </c>
+      <c r="I12" s="16">
+        <v>0</v>
+      </c>
+      <c r="J12" s="16">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9">
+        <v>0</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0</v>
+      </c>
+      <c r="M12" s="9">
         <v>0</v>
       </c>
       <c r="N12" s="12">
@@ -4110,234 +3663,203 @@
       <c r="R12" s="12">
         <v>0</v>
       </c>
-      <c r="S12" s="17">
-        <v>0</v>
-      </c>
-      <c r="T12" s="17">
-        <v>0</v>
-      </c>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="21"/>
+      <c r="S12" s="16">
+        <v>0</v>
+      </c>
+      <c r="T12" s="16">
+        <v>0</v>
+      </c>
       <c r="Y12" s="10"/>
-      <c r="Z12" s="21"/>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="21"/>
-      <c r="AC12" s="21"/>
-      <c r="AD12" s="21"/>
-      <c r="AE12" s="21"/>
-      <c r="AF12" s="21"/>
-      <c r="AG12" s="21"/>
-      <c r="AH12" s="21"/>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>315</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <f>(D7+D9)*Parameters!$O$30+D8*Parameters!$O$31+D10*Parameters!$O$32+D11*Parameters!$O$15+D12*Parameters!$O$16</f>
         <v>0.03</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <f>(E7+E9)*Parameters!$O$30+E8*Parameters!$O$31+E10*Parameters!$O$32+E11*Parameters!$O$15+E12*Parameters!$O$16</f>
         <v>0.03</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="16">
         <f>(F7+F9)*Parameters!$O$30+F8*Parameters!$O$31+F10*Parameters!$O$32+F11*Parameters!$O$15+F12*Parameters!$O$16</f>
         <v>0.03</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="16">
         <f>(G7+G9)*Parameters!$O$30+G8*Parameters!$O$31+G10*Parameters!$O$32+G11*Parameters!$O$15+G12*Parameters!$O$16</f>
         <v>2.9791501244684441E-2</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="16">
         <f>(H7+H9)*Parameters!$O$30+H8*Parameters!$O$31+H10*Parameters!$O$32+H11*Parameters!$O$15+H12*Parameters!$O$16</f>
         <v>2.9756292854192387E-2</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="16">
         <f>(I7+I9)*Parameters!$O$30+I8*Parameters!$O$31+I10*Parameters!$O$32+I11*Parameters!$O$15+I12*Parameters!$O$16</f>
         <v>3.0552454135509274E-2</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="16">
         <f>(J7+J9)*Parameters!$O$30+J8*Parameters!$O$31+J10*Parameters!$O$32+J11*Parameters!$O$15+J12*Parameters!$O$16</f>
         <v>2.9397194168044868E-2</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="16">
         <f>(K7+K9)*Parameters!$O$30+K8*Parameters!$O$31+K10*Parameters!$O$32+K11*Parameters!$O$15+K12*Parameters!$O$16</f>
         <v>3.0621863216685027E-2</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="16">
         <f>(L7+L9)*Parameters!$O$30+L8*Parameters!$O$31+L10*Parameters!$O$32+L11*Parameters!$O$15+L12*Parameters!$O$16</f>
         <v>2.8456430440886006E-2</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="16">
         <f>(M7+M9)*Parameters!$O$30+M8*Parameters!$O$31+M10*Parameters!$O$32+M11*Parameters!$O$15+M12*Parameters!$O$16</f>
         <v>3.0602017378064218E-2</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13" s="16">
         <f>(N7+N9)*Parameters!$O$30+N8*Parameters!$O$31+N10*Parameters!$O$32+N11*Parameters!$O$15+N12*Parameters!$O$16</f>
         <v>3.0948774065621982E-2</v>
       </c>
-      <c r="O13" s="17">
+      <c r="O13" s="16">
         <f>(O7+O9)*Parameters!$O$30+O8*Parameters!$O$31+O10*Parameters!$O$32+O11*Parameters!$O$15+O12*Parameters!$O$16</f>
         <v>3.1063198360634463E-2</v>
       </c>
-      <c r="P13" s="17">
+      <c r="P13" s="16">
         <f>(P7+P9)*Parameters!$O$30+P8*Parameters!$O$31+P10*Parameters!$O$32+P11*Parameters!$O$15+P12*Parameters!$O$16</f>
         <v>2.7045657175301968E-2</v>
       </c>
-      <c r="Q13" s="17">
+      <c r="Q13" s="16">
         <f>(Q7+Q9)*Parameters!$O$30+Q8*Parameters!$O$31+Q10*Parameters!$O$32+Q11*Parameters!$O$15+Q12*Parameters!$O$16</f>
         <v>2.4712807006981814E-2</v>
       </c>
-      <c r="R13" s="17">
+      <c r="R13" s="16">
         <f>(R7+R9)*Parameters!$O$30+R8*Parameters!$O$31+R10*Parameters!$O$32+R11*Parameters!$O$15+R12*Parameters!$O$16</f>
         <v>2.6680335917312663E-2</v>
       </c>
-      <c r="S13" s="17">
+      <c r="S13" s="16">
         <f>(S7+S9)*Parameters!$O$30+S8*Parameters!$O$31+S10*Parameters!$O$32+S11*Parameters!$O$15+S12*Parameters!$O$16</f>
         <v>3.0901481061503838E-2</v>
       </c>
-      <c r="T13" s="17">
+      <c r="T13" s="16">
         <f>(T7+T9)*Parameters!$O$30+T8*Parameters!$O$31+T10*Parameters!$O$32+T11*Parameters!$O$15+T12*Parameters!$O$16</f>
         <v>3.0604089508049784E-2</v>
       </c>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21"/>
-      <c r="AC13" s="21"/>
-      <c r="AD13" s="21"/>
-      <c r="AE13" s="21"/>
-      <c r="AF13" s="21"/>
-      <c r="AG13" s="21"/>
-      <c r="AH13" s="21"/>
-    </row>
-    <row r="14" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="26"/>
+    </row>
+    <row r="14" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>318</v>
       </c>
       <c r="C14">
         <v>11</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <f>D8*Parameters!$O$45+SUM(D11:D12)*Parameters!$O$44</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="17">
         <f>E8*Parameters!$O$45+SUM(E11:E12)*Parameters!$O$44</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <f>F8*Parameters!$O$45+SUM(F11:F12)*Parameters!$O$44</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="17">
         <f>G8*Parameters!$O$45+SUM(G11:G12)*Parameters!$O$44</f>
         <v>1.2729577792850938E-3</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="17">
         <f>H8*Parameters!$O$45+SUM(H11:H12)*Parameters!$O$44</f>
         <v>6.7879079817428076E-4</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="17">
         <f>I8*Parameters!$O$45+SUM(I11:I12)*Parameters!$O$44</f>
         <v>6.5055051344153317E-4</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="17">
         <f>J8*Parameters!$O$45+SUM(J11:J12)*Parameters!$O$44</f>
         <v>6.4725448970392608E-3</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="17">
         <f>K8*Parameters!$O$45+SUM(K11:K12)*Parameters!$O$44</f>
         <v>1.8015817858719522E-3</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="17">
         <f>L8*Parameters!$O$45+SUM(L11:L12)*Parameters!$O$44</f>
         <v>1.3198629937924077E-3</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="17">
         <f>M8*Parameters!$O$45+SUM(M11:M12)*Parameters!$O$44</f>
         <v>1.8785714867599146E-3</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="17">
         <f>N8*Parameters!$O$45+SUM(N11:N12)*Parameters!$O$44</f>
         <v>2.3420795246246036E-4</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O14" s="17">
         <f>O8*Parameters!$O$45+SUM(O11:O12)*Parameters!$O$44</f>
         <v>1.0387597910888627E-4</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="17">
         <f>P8*Parameters!$O$45+SUM(P11:P12)*Parameters!$O$44</f>
         <v>4.4149500283892267E-3</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="Q14" s="17">
         <f>Q8*Parameters!$O$45+SUM(Q11:Q12)*Parameters!$O$44</f>
         <v>1.3718017964808238E-3</v>
       </c>
-      <c r="R14" s="18">
+      <c r="R14" s="17">
         <f>R8*Parameters!$O$45+SUM(R11:R12)*Parameters!$O$44</f>
         <v>2.0005167958656333E-3</v>
       </c>
-      <c r="S14" s="18">
+      <c r="S14" s="17">
         <f>S8*Parameters!$O$45+SUM(S11:S12)*Parameters!$O$44</f>
         <v>4.7879353978052549E-4</v>
       </c>
-      <c r="T14" s="18">
+      <c r="T14" s="17">
         <f>T8*Parameters!$O$45+SUM(T11:T12)*Parameters!$O$44</f>
         <v>1.0369724529819564E-3</v>
       </c>
-      <c r="X14" s="17"/>
-      <c r="Z14" s="17"/>
-      <c r="AG14" s="21"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A15" s="26"/>
+      <c r="X14" s="16"/>
+      <c r="Z14" s="16"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>425</v>
       </c>
       <c r="C15">
         <v>12</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="21">
         <v>4.6511627906976737E-2</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="21">
         <v>2.8901734104046249E-2</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="21">
         <v>5.3113553113553022E-2</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="21">
         <v>2.0795857272247545E-2</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="18">
         <v>2.0795857272247545E-2</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="18">
         <v>7.0515726809881232E-2</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15" s="21">
         <v>4.8303366664342595E-2</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="21">
         <v>6.4810323210917051E-2</v>
       </c>
-      <c r="L15" s="24">
+      <c r="L15" s="21">
         <v>1.9604636911718556E-2</v>
       </c>
-      <c r="M15" s="24">
+      <c r="M15" s="21">
         <v>5.0137074654958078E-2</v>
       </c>
       <c r="N15" s="10">
@@ -4355,51 +3877,47 @@
       <c r="R15" s="10">
         <v>3.9141886047995844E-2</v>
       </c>
-      <c r="S15" s="24">
+      <c r="S15" s="21">
         <v>7.0515726809881232E-2</v>
       </c>
-      <c r="T15" s="24">
+      <c r="T15" s="21">
         <v>2.0795857272247545E-2</v>
       </c>
-      <c r="V15" s="21"/>
-      <c r="X15" s="17"/>
-      <c r="Z15" s="17"/>
-      <c r="AG15" s="21"/>
-      <c r="AH15" s="21"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A16" s="26"/>
+      <c r="X15" s="16"/>
+      <c r="Z15" s="16"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.35">
       <c r="C16">
         <v>13</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <v>2.6578073089701011E-2</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="21">
         <v>9.2485549132947917E-2</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="21">
         <v>9.3406593406593588E-2</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="21">
         <v>3.9553134087838136E-2</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="18">
         <v>3.9553134087838136E-2</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="18">
         <v>7.8778404269144994E-2</v>
       </c>
-      <c r="J16" s="24">
+      <c r="J16" s="21">
         <v>9.5433005590842765E-2</v>
       </c>
-      <c r="K16" s="24">
+      <c r="K16" s="21">
         <v>6.9113357949129109E-2</v>
       </c>
-      <c r="L16" s="24">
+      <c r="L16" s="21">
         <v>4.9279071274079059E-2</v>
       </c>
-      <c r="M16" s="24">
+      <c r="M16" s="21">
         <v>7.5400613569254163E-2</v>
       </c>
       <c r="N16" s="10">
@@ -4417,51 +3935,47 @@
       <c r="R16" s="10">
         <v>7.3524504056198092E-2</v>
       </c>
-      <c r="S16" s="24">
+      <c r="S16" s="21">
         <v>7.8778404269144994E-2</v>
       </c>
-      <c r="T16" s="24">
+      <c r="T16" s="21">
         <v>3.9553134087838136E-2</v>
       </c>
-      <c r="V16" s="21"/>
-      <c r="X16" s="17"/>
-      <c r="Z16" s="17"/>
-      <c r="AG16" s="21"/>
-      <c r="AH16" s="21"/>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A17" s="26"/>
+      <c r="X16" s="16"/>
+      <c r="Z16" s="16"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C17">
         <v>14</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="21">
         <v>6.3122923588039948E-2</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="21">
         <v>2.3121387283237E-2</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="21">
         <v>6.7765567765567733E-2</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="21">
         <v>6.0246587068673672E-3</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="18">
         <v>6.0246587068673672E-3</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="18">
         <v>8.7860626315211833E-3</v>
       </c>
-      <c r="J17" s="24">
+      <c r="J17" s="21">
         <v>9.7333253148368493E-2</v>
       </c>
-      <c r="K17" s="24">
+      <c r="K17" s="21">
         <v>3.083252560136587E-2</v>
       </c>
-      <c r="L17" s="24">
+      <c r="L17" s="21">
         <v>7.9387197805777604E-2</v>
       </c>
-      <c r="M17" s="24">
+      <c r="M17" s="21">
         <v>5.045604968168136E-2</v>
       </c>
       <c r="N17" s="10">
@@ -4479,51 +3993,47 @@
       <c r="R17" s="10">
         <v>0.15044857011318213</v>
       </c>
-      <c r="S17" s="24">
+      <c r="S17" s="21">
         <v>8.7860626315211833E-3</v>
       </c>
-      <c r="T17" s="24">
+      <c r="T17" s="21">
         <v>6.0246587068673672E-3</v>
       </c>
-      <c r="V17" s="21"/>
-      <c r="X17" s="17"/>
-      <c r="Z17" s="17"/>
-      <c r="AG17" s="21"/>
-      <c r="AH17" s="21"/>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A18" s="26"/>
+      <c r="X17" s="16"/>
+      <c r="Z17" s="16"/>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C18">
         <v>15</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="21">
         <v>3.3222591362126255E-2</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="21">
         <v>5.7803468208092498E-2</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="21">
         <v>0.10439560439560426</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="21">
         <v>9.0601885577154592E-3</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="18">
         <v>9.0601885577154592E-3</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="18">
         <v>2.6012161455308436E-2</v>
       </c>
-      <c r="J18" s="24">
+      <c r="J18" s="21">
         <v>8.8366702039211695E-2</v>
       </c>
-      <c r="K18" s="24">
+      <c r="K18" s="21">
         <v>5.090798426561137E-2</v>
       </c>
-      <c r="L18" s="24">
+      <c r="L18" s="21">
         <v>3.0039981804061894E-2</v>
       </c>
-      <c r="M18" s="24">
+      <c r="M18" s="21">
         <v>6.8945081585585141E-2</v>
       </c>
       <c r="N18" s="10">
@@ -4541,51 +4051,47 @@
       <c r="R18" s="10">
         <v>5.4831237214669953E-2</v>
       </c>
-      <c r="S18" s="24">
+      <c r="S18" s="21">
         <v>2.6012161455308436E-2</v>
       </c>
-      <c r="T18" s="24">
+      <c r="T18" s="21">
         <v>9.0601885577154592E-3</v>
       </c>
-      <c r="V18" s="21"/>
-      <c r="X18" s="17"/>
-      <c r="Z18" s="17"/>
-      <c r="AG18" s="21"/>
-      <c r="AH18" s="21"/>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A19" s="26"/>
+      <c r="X18" s="16"/>
+      <c r="Z18" s="16"/>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C19">
         <v>16</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="21">
         <v>4.9833887043189203E-2</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="21">
         <v>6.9364161849710809E-2</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="21">
         <v>0.11172161172161184</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="21">
         <v>2.0934762554189138E-2</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="18">
         <v>2.0934762554189138E-2</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="18">
         <v>8.4163158291113357E-2</v>
       </c>
-      <c r="J19" s="24">
+      <c r="J19" s="21">
         <v>0.12834582284751955</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="21">
         <v>9.7636331070991914E-2</v>
       </c>
-      <c r="L19" s="24">
+      <c r="L19" s="21">
         <v>0.16575348992415107</v>
       </c>
-      <c r="M19" s="24">
+      <c r="M19" s="21">
         <v>4.5650711616759328E-2</v>
       </c>
       <c r="N19" s="10">
@@ -4603,51 +4109,47 @@
       <c r="R19" s="10">
         <v>8.5503817536255189E-2</v>
       </c>
-      <c r="S19" s="24">
+      <c r="S19" s="21">
         <v>8.4163158291113357E-2</v>
       </c>
-      <c r="T19" s="24">
+      <c r="T19" s="21">
         <v>2.0934762554189138E-2</v>
       </c>
-      <c r="V19" s="21"/>
-      <c r="X19" s="17"/>
-      <c r="Z19" s="17"/>
-      <c r="AG19" s="21"/>
-      <c r="AH19" s="21"/>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A20" s="26"/>
+      <c r="X19" s="16"/>
+      <c r="Z19" s="16"/>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C20">
         <v>17</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="21">
         <v>5.3156146179402113E-2</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="21">
         <v>8.0924855491329592E-2</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="21">
         <v>4.9450549450549462E-2</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="21">
         <v>6.4876287882916453E-2</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="18">
         <v>6.4876287882916453E-2</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="18">
         <v>7.7903088666154502E-2</v>
       </c>
-      <c r="J20" s="24">
+      <c r="J20" s="21">
         <v>5.4603425620141449E-2</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="21">
         <v>4.8818165535495957E-2</v>
       </c>
-      <c r="L20" s="24">
+      <c r="L20" s="21">
         <v>4.0222846888260659E-2</v>
       </c>
-      <c r="M20" s="24">
+      <c r="M20" s="21">
         <v>4.4737697384424131E-2</v>
       </c>
       <c r="N20" s="10">
@@ -4665,51 +4167,47 @@
       <c r="R20" s="10">
         <v>6.1881147631844297E-2</v>
       </c>
-      <c r="S20" s="24">
+      <c r="S20" s="21">
         <v>7.7903088666154502E-2</v>
       </c>
-      <c r="T20" s="24">
+      <c r="T20" s="21">
         <v>6.4876287882916453E-2</v>
       </c>
-      <c r="V20" s="21"/>
-      <c r="X20" s="17"/>
-      <c r="Z20" s="17"/>
-      <c r="AG20" s="21"/>
-      <c r="AH20" s="21"/>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A21" s="26"/>
+      <c r="X20" s="16"/>
+      <c r="Z20" s="16"/>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C21">
         <v>18</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="21">
         <v>0.10963455149501669</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="21">
         <v>9.8265895953757315E-2</v>
       </c>
-      <c r="F21" s="24">
+      <c r="F21" s="21">
         <v>4.9450549450549462E-2</v>
       </c>
-      <c r="G21" s="24">
+      <c r="G21" s="21">
         <v>3.8438142064387962E-2</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="18">
         <v>3.8438142064387962E-2</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="18">
         <v>3.9278868235035881E-2</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J21" s="21">
         <v>5.1734533197739185E-2</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="21">
         <v>4.0921109345930434E-2</v>
       </c>
-      <c r="L21" s="24">
+      <c r="L21" s="21">
         <v>3.6855775994899469E-2</v>
       </c>
-      <c r="M21" s="24">
+      <c r="M21" s="21">
         <v>5.9211658302914298E-2</v>
       </c>
       <c r="N21" s="10">
@@ -4727,51 +4225,47 @@
       <c r="R21" s="10">
         <v>3.7278210033879947E-2</v>
       </c>
-      <c r="S21" s="24">
+      <c r="S21" s="21">
         <v>3.9278868235035881E-2</v>
       </c>
-      <c r="T21" s="24">
+      <c r="T21" s="21">
         <v>3.8438142064387962E-2</v>
       </c>
-      <c r="V21" s="21"/>
-      <c r="X21" s="17"/>
-      <c r="Z21" s="17"/>
-      <c r="AG21" s="21"/>
-      <c r="AH21" s="21"/>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A22" s="26"/>
+      <c r="X21" s="16"/>
+      <c r="Z21" s="16"/>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C22">
         <v>19</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="21">
         <v>7.9734219269103151E-2</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="21">
         <v>1.15606936416185E-2</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="21">
         <v>6.4102564102564166E-2</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="21">
         <v>1.4506213339541585E-2</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="18">
         <v>1.4506213339541585E-2</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="18">
         <v>2.9541901600929375E-2</v>
       </c>
-      <c r="J22" s="24">
+      <c r="J22" s="21">
         <v>1.6952571526064025E-2</v>
       </c>
-      <c r="K22" s="24">
+      <c r="K22" s="21">
         <v>1.1518892991521517E-2</v>
       </c>
-      <c r="L22" s="24">
+      <c r="L22" s="21">
         <v>1.642635709135969E-2</v>
       </c>
-      <c r="M22" s="24">
+      <c r="M22" s="21">
         <v>2.2620184070776251E-2</v>
       </c>
       <c r="N22" s="10">
@@ -4789,51 +4283,47 @@
       <c r="R22" s="10">
         <v>1.0861532240785345E-2</v>
       </c>
-      <c r="S22" s="24">
+      <c r="S22" s="21">
         <v>2.9541901600929375E-2</v>
       </c>
-      <c r="T22" s="24">
+      <c r="T22" s="21">
         <v>1.4506213339541585E-2</v>
       </c>
-      <c r="V22" s="21"/>
-      <c r="X22" s="17"/>
-      <c r="Z22" s="17"/>
-      <c r="AG22" s="21"/>
-      <c r="AH22" s="21"/>
-    </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A23" s="26"/>
+      <c r="X22" s="16"/>
+      <c r="Z22" s="16"/>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C23">
         <v>20</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="21">
         <v>0.11627906976744164</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="21">
         <v>1.7341040462427747E-2</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="21">
         <v>3.1135531135531101E-2</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="21">
         <v>0.12162868546728456</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="18">
         <v>0.12162868546728456</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="18">
         <v>6.6217625366231325E-2</v>
       </c>
-      <c r="J23" s="24">
+      <c r="J23" s="21">
         <v>8.9856163564373134E-2</v>
       </c>
-      <c r="K23" s="24">
+      <c r="K23" s="21">
         <v>8.2014518099633213E-2</v>
       </c>
-      <c r="L23" s="24">
+      <c r="L23" s="21">
         <v>4.11510664318359E-2</v>
       </c>
-      <c r="M23" s="24">
+      <c r="M23" s="21">
         <v>9.3949164507290683E-2</v>
       </c>
       <c r="N23" s="10">
@@ -4851,51 +4341,47 @@
       <c r="R23" s="10">
         <v>8.7378485471246728E-2</v>
       </c>
-      <c r="S23" s="24">
+      <c r="S23" s="21">
         <v>6.6217625366231325E-2</v>
       </c>
-      <c r="T23" s="24">
+      <c r="T23" s="21">
         <v>0.12162868546728456</v>
       </c>
-      <c r="V23" s="21"/>
-      <c r="X23" s="17"/>
-      <c r="Z23" s="17"/>
-      <c r="AG23" s="21"/>
-      <c r="AH23" s="21"/>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A24" s="26"/>
+      <c r="X23" s="16"/>
+      <c r="Z23" s="16"/>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C24">
         <v>21</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="21">
         <v>5.6478405315614572E-2</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="21">
         <v>0.12138728323699439</v>
       </c>
-      <c r="F24" s="24">
+      <c r="F24" s="21">
         <v>5.4945054945054798E-2</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="21">
         <v>0.15223854250977051</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="18">
         <v>0.15223854250977051</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="18">
         <v>4.8266044064900065E-2</v>
       </c>
-      <c r="J24" s="24">
+      <c r="J24" s="21">
         <v>4.3218218151357075E-2</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="21">
         <v>3.3429830747133099E-2</v>
       </c>
-      <c r="L24" s="24">
+      <c r="L24" s="21">
         <v>2.1187620016391483E-2</v>
       </c>
-      <c r="M24" s="24">
+      <c r="M24" s="21">
         <v>4.960049057838329E-2</v>
       </c>
       <c r="N24" s="10">
@@ -4913,51 +4399,47 @@
       <c r="R24" s="10">
         <v>6.1256574626210217E-2</v>
       </c>
-      <c r="S24" s="24">
+      <c r="S24" s="21">
         <v>4.8266044064900065E-2</v>
       </c>
-      <c r="T24" s="24">
+      <c r="T24" s="21">
         <v>0.15223854250977051</v>
       </c>
-      <c r="V24" s="21"/>
-      <c r="X24" s="17"/>
-      <c r="Z24" s="17"/>
-      <c r="AG24" s="21"/>
-      <c r="AH24" s="21"/>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A25" s="26"/>
+      <c r="X24" s="16"/>
+      <c r="Z24" s="16"/>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C25">
         <v>22</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="21">
         <v>5.9800664451827058E-2</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="21">
         <v>7.5144508670520208E-2</v>
       </c>
-      <c r="F25" s="24">
+      <c r="F25" s="21">
         <v>6.4102564102564166E-2</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25" s="21">
         <v>3.7758141606185416E-2</v>
       </c>
-      <c r="H25" s="19">
+      <c r="H25" s="18">
         <v>3.7758141606185416E-2</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="18">
         <v>3.9950301880079232E-2</v>
       </c>
-      <c r="J25" s="24">
+      <c r="J25" s="21">
         <v>6.1822763984065054E-2</v>
       </c>
-      <c r="K25" s="24">
+      <c r="K25" s="21">
         <v>4.8192291618374218E-2</v>
       </c>
-      <c r="L25" s="24">
+      <c r="L25" s="21">
         <v>2.4990526173179695E-2</v>
       </c>
-      <c r="M25" s="24">
+      <c r="M25" s="21">
         <v>7.1695027859654051E-2</v>
       </c>
       <c r="N25" s="10">
@@ -4975,52 +4457,48 @@
       <c r="R25" s="10">
         <v>6.1808996461924906E-2</v>
       </c>
-      <c r="S25" s="24">
+      <c r="S25" s="21">
         <v>3.9950301880079232E-2</v>
       </c>
-      <c r="T25" s="24">
+      <c r="T25" s="21">
         <v>3.7758141606185416E-2</v>
       </c>
-      <c r="V25" s="21"/>
-      <c r="X25" s="17"/>
-      <c r="Z25" s="17"/>
-      <c r="AA25" s="19"/>
-      <c r="AG25" s="21"/>
-      <c r="AH25" s="21"/>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A26" s="26"/>
+      <c r="X25" s="16"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="18"/>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C26">
         <v>23</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="21">
         <v>3.3222591362126255E-2</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="21">
         <v>7.5144508670520208E-2</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="21">
         <v>4.3956043956043939E-2</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="21">
         <v>3.0700353536597051E-2</v>
       </c>
-      <c r="H26" s="19">
+      <c r="H26" s="18">
         <v>3.0700353536597051E-2</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="18">
         <v>1.1150251240384709E-2</v>
       </c>
-      <c r="J26" s="24">
+      <c r="J26" s="21">
         <v>4.9411886819540479E-2</v>
       </c>
-      <c r="K26" s="24">
+      <c r="K26" s="21">
         <v>4.1085517177774269E-2</v>
       </c>
-      <c r="L26" s="24">
+      <c r="L26" s="21">
         <v>2.2319782918030721E-2</v>
       </c>
-      <c r="M26" s="24">
+      <c r="M26" s="21">
         <v>7.683955657630101E-2</v>
       </c>
       <c r="N26" s="10">
@@ -5038,52 +4516,48 @@
       <c r="R26" s="10">
         <v>3.5025280658121799E-2</v>
       </c>
-      <c r="S26" s="24">
+      <c r="S26" s="21">
         <v>1.1150251240384709E-2</v>
       </c>
-      <c r="T26" s="24">
+      <c r="T26" s="21">
         <v>3.0700353536597051E-2</v>
       </c>
-      <c r="V26" s="21"/>
-      <c r="X26" s="17"/>
-      <c r="Z26" s="17"/>
-      <c r="AA26" s="19"/>
-      <c r="AG26" s="21"/>
-      <c r="AH26" s="21"/>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A27" s="26"/>
+      <c r="X26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="18"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C27">
         <v>24</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="21">
         <v>3.9867109634551499E-2</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="21">
         <v>7.5144508670520208E-2</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="21">
         <v>0.11904761904761897</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="21">
         <v>6.1643915138483538E-2</v>
       </c>
-      <c r="H27" s="19">
+      <c r="H27" s="18">
         <v>6.1643915138483538E-2</v>
       </c>
-      <c r="I27" s="19">
+      <c r="I27" s="18">
         <v>2.6760602976923301E-2</v>
       </c>
-      <c r="J27" s="24">
+      <c r="J27" s="21">
         <v>8.7148295811977472E-2</v>
       </c>
-      <c r="K27" s="24">
+      <c r="K27" s="21">
         <v>5.673714276930733E-2</v>
       </c>
-      <c r="L27" s="24">
+      <c r="L27" s="21">
         <v>3.0999698497264888E-2</v>
       </c>
-      <c r="M27" s="24">
+      <c r="M27" s="21">
         <v>7.1716919471214266E-2</v>
       </c>
       <c r="N27" s="10">
@@ -5101,52 +4575,48 @@
       <c r="R27" s="10">
         <v>7.2142327046148425E-2</v>
       </c>
-      <c r="S27" s="24">
+      <c r="S27" s="21">
         <v>2.6760602976923301E-2</v>
       </c>
-      <c r="T27" s="24">
+      <c r="T27" s="21">
         <v>6.1643915138483538E-2</v>
       </c>
-      <c r="V27" s="21"/>
-      <c r="X27" s="17"/>
-      <c r="Z27" s="19"/>
-      <c r="AA27" s="19"/>
-      <c r="AG27" s="21"/>
-      <c r="AH27" s="21"/>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A28" s="26"/>
+      <c r="X27" s="16"/>
+      <c r="Z27" s="18"/>
+      <c r="AA27" s="18"/>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C28">
         <v>25</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="21">
         <v>2.9900332225913609E-2</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="21">
         <v>2.3121387283237E-2</v>
       </c>
-      <c r="F28" s="24">
-        <v>0</v>
-      </c>
-      <c r="G28" s="24">
+      <c r="F28" s="21">
+        <v>0</v>
+      </c>
+      <c r="G28" s="21">
         <v>7.552867215490278E-3</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="18">
         <v>7.552867215490278E-3</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="18">
         <v>4.7440983482594089E-2</v>
       </c>
-      <c r="J28" s="24">
+      <c r="J28" s="21">
         <v>3.5551249963842728E-2</v>
       </c>
-      <c r="K28" s="24">
+      <c r="K28" s="21">
         <v>1.3143352259556604E-2</v>
       </c>
-      <c r="L28" s="24">
+      <c r="L28" s="21">
         <v>8.3301753910598984E-3</v>
       </c>
-      <c r="M28" s="24">
+      <c r="M28" s="21">
         <v>1.7206806686316977E-2</v>
       </c>
       <c r="N28" s="10">
@@ -5164,51 +4634,47 @@
       <c r="R28" s="10">
         <v>1.1701612886821811E-2</v>
       </c>
-      <c r="S28" s="24">
+      <c r="S28" s="21">
         <v>4.7440983482594089E-2</v>
       </c>
-      <c r="T28" s="24">
+      <c r="T28" s="21">
         <v>7.552867215490278E-3</v>
       </c>
-      <c r="V28" s="21"/>
-      <c r="Z28" s="19"/>
-      <c r="AA28" s="19"/>
-      <c r="AG28" s="21"/>
-      <c r="AH28" s="21"/>
-    </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A29" s="26"/>
+      <c r="Z28" s="18"/>
+      <c r="AA28" s="18"/>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C29">
         <v>26</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="21">
         <v>9.6345514950165953E-2</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="21">
         <v>8.6705202312138532E-2</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="21">
         <v>3.6630036630036625E-2</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="21">
         <v>0.34927561540518987</v>
       </c>
-      <c r="H29" s="19">
+      <c r="H29" s="18">
         <v>0.34927561540518987</v>
       </c>
-      <c r="I29" s="19">
+      <c r="I29" s="18">
         <v>0.15737357680461606</v>
       </c>
-      <c r="J29" s="24">
+      <c r="J29" s="21">
         <v>1.435832264732525E-2</v>
       </c>
-      <c r="K29" s="24">
+      <c r="K29" s="21">
         <v>0.24576268266157214</v>
       </c>
-      <c r="L29" s="24">
+      <c r="L29" s="21">
         <v>0.3126383291459775</v>
       </c>
-      <c r="M29" s="24">
+      <c r="M29" s="21">
         <v>0.10571579176456389</v>
       </c>
       <c r="N29" s="10">
@@ -5226,51 +4692,47 @@
       <c r="R29" s="10">
         <v>7.1111448247764136E-2</v>
       </c>
-      <c r="S29" s="24">
+      <c r="S29" s="21">
         <v>0.15737357680461606</v>
       </c>
-      <c r="T29" s="24">
+      <c r="T29" s="21">
         <v>0.34927561540518987</v>
       </c>
-      <c r="V29" s="21"/>
-      <c r="Z29" s="19"/>
-      <c r="AA29" s="19"/>
-      <c r="AG29" s="21"/>
-      <c r="AH29" s="21"/>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A30" s="26"/>
+      <c r="Z29" s="18"/>
+      <c r="AA29" s="18"/>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C30">
         <v>27</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="21">
         <v>6.3122923588039948E-2</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="21">
         <v>4.6242774566473958E-2</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="21">
         <v>2.3809523809523791E-2</v>
       </c>
-      <c r="G30" s="24">
+      <c r="G30" s="21">
         <v>1.1490593860432075E-2</v>
       </c>
-      <c r="H30" s="19">
+      <c r="H30" s="18">
         <v>1.1490593860432075E-2</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="18">
         <v>0.14828144717705544</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J30" s="21">
         <v>1.0896736253142265E-2</v>
       </c>
-      <c r="K30" s="24">
+      <c r="K30" s="21">
         <v>4.8540789594953365E-2</v>
       </c>
-      <c r="L30" s="24">
+      <c r="L30" s="21">
         <v>8.6141586430278499E-2</v>
       </c>
-      <c r="M30" s="24">
+      <c r="M30" s="21">
         <v>7.8799353347565243E-2</v>
       </c>
       <c r="N30" s="10">
@@ -5288,55 +4750,51 @@
       <c r="R30" s="10">
         <v>4.948430975449105E-2</v>
       </c>
-      <c r="S30" s="24">
+      <c r="S30" s="21">
         <v>0.14828144717705544</v>
       </c>
-      <c r="T30" s="24">
+      <c r="T30" s="21">
         <v>1.1490593860432075E-2</v>
       </c>
-      <c r="V30" s="21"/>
-      <c r="X30" s="19"/>
-      <c r="Z30" s="19"/>
-      <c r="AA30" s="19"/>
-      <c r="AG30" s="21"/>
-      <c r="AH30" s="21"/>
-    </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A31" s="26"/>
+      <c r="X30" s="18"/>
+      <c r="Z30" s="18"/>
+      <c r="AA30" s="18"/>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>426</v>
       </c>
       <c r="C31">
         <v>28</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="21">
         <v>4.3189368770764264E-2</v>
       </c>
-      <c r="E31" s="24">
+      <c r="E31" s="21">
         <v>1.7341040462427747E-2</v>
       </c>
-      <c r="F31" s="24">
+      <c r="F31" s="21">
         <v>3.2967032967032926E-2</v>
       </c>
-      <c r="G31" s="24">
+      <c r="G31" s="21">
         <v>1.3522040794863115E-2</v>
       </c>
-      <c r="H31" s="19">
+      <c r="H31" s="18">
         <v>1.3522040794863115E-2</v>
       </c>
-      <c r="I31" s="19">
+      <c r="I31" s="18">
         <v>3.9579795048126885E-2</v>
       </c>
-      <c r="J31" s="24">
+      <c r="J31" s="21">
         <v>2.6663682170146974E-2</v>
       </c>
-      <c r="K31" s="24">
+      <c r="K31" s="21">
         <v>1.6535185100732503E-2</v>
       </c>
-      <c r="L31" s="24">
+      <c r="L31" s="21">
         <v>1.467185730167324E-2</v>
       </c>
-      <c r="M31" s="24">
+      <c r="M31" s="21">
         <v>1.7317818342357731E-2</v>
       </c>
       <c r="N31" s="10">
@@ -5354,16 +4812,14 @@
       <c r="R31" s="10">
         <v>3.662005997246022E-2</v>
       </c>
-      <c r="S31" s="24">
+      <c r="S31" s="21">
         <v>3.9579795048126885E-2</v>
       </c>
-      <c r="T31" s="24">
+      <c r="T31" s="21">
         <v>1.3522040794863115E-2</v>
       </c>
-      <c r="AG31" s="21"/>
-    </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A32" s="26"/>
+    </row>
+    <row r="32" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>424</v>
       </c>
@@ -5423,77 +4879,74 @@
       </c>
       <c r="U32" s="12"/>
       <c r="V32" s="12"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="22"/>
-      <c r="Z32" s="22"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="26"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E35" s="24"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="D36" s="25"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="25"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E37" s="24"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E38" s="24"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E39" s="24"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E40" s="24"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E41" s="24"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E42" s="24"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E43" s="24"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E44" s="24"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E45" s="24"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E46" s="24"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E47" s="24"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E48" s="24"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E35" s="21"/>
+    </row>
+    <row r="36" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="D36" s="22"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E37" s="21"/>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E38" s="21"/>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E39" s="21"/>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E40" s="21"/>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E42" s="21"/>
+    </row>
+    <row r="43" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E43" s="21"/>
+    </row>
+    <row r="44" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E44" s="21"/>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E45" s="21"/>
+    </row>
+    <row r="46" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E46" s="21"/>
+    </row>
+    <row r="47" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E47" s="21"/>
+    </row>
+    <row r="48" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E48" s="21"/>
     </row>
     <row r="49" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E49" s="24"/>
+      <c r="E49" s="21"/>
     </row>
     <row r="50" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E50" s="24"/>
+      <c r="E50" s="21"/>
     </row>
     <row r="51" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E51" s="24"/>
+      <c r="E51" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8102,79 +7555,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="T4:W5 J4:J5 L4:R13 C4:I14 L14:W14 C15:W30">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S4:S5">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T6:W13 J6:J13">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S6:S13">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K5">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6:K13">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31:W32">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33:W35">
+  <conditionalFormatting sqref="C4:W35">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -8265,7 +7646,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" t="s">
         <v>377</v>
       </c>
       <c r="G3" t="s">
@@ -8303,7 +7684,7 @@
       <c r="C4">
         <v>0.25</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" t="s">
         <v>377</v>
       </c>
       <c r="E4" s="3"/>
@@ -8343,7 +7724,7 @@
       <c r="C5">
         <v>8314</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" t="s">
         <v>308</v>
       </c>
       <c r="E5" s="3"/>
@@ -8383,7 +7764,7 @@
       <c r="C6">
         <v>298.14999999999998</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" t="s">
         <v>376</v>
       </c>
       <c r="E6" s="3"/>
@@ -8542,7 +7923,7 @@
       <c r="N9" t="s">
         <v>316</v>
       </c>
-      <c r="O9" s="15">
+      <c r="O9" s="14">
         <f>(O3+O5)*O$30+O4*O$31+O6*O$32+O7*O$33+O8*O$29</f>
         <v>3.0022017879448977E-2</v>
       </c>
@@ -8591,7 +7972,7 @@
       <c r="N10" t="s">
         <v>319</v>
       </c>
-      <c r="O10" s="15">
+      <c r="O10" s="14">
         <f>O4*O$45+(O7+O8)*O$44</f>
         <v>2.0313990759434084E-3</v>
       </c>
@@ -8762,7 +8143,7 @@
       <c r="J14" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="21" t="s">
+      <c r="K14" t="s">
         <v>436</v>
       </c>
       <c r="M14" t="s">
@@ -8888,7 +8269,7 @@
       <c r="N17" t="s">
         <v>328</v>
       </c>
-      <c r="O17" s="15">
+      <c r="O17" s="14">
         <f>(O11+O13)*O$30+O12*O$31+O14*O$32+O15*O$33+O16*O$29</f>
         <v>2.9756292854192387E-2</v>
       </c>
@@ -8933,7 +8314,7 @@
       <c r="N18" t="s">
         <v>330</v>
       </c>
-      <c r="O18" s="15">
+      <c r="O18" s="14">
         <f>O12*O$45+(O15+O16)*O$44</f>
         <v>6.7879079817428076E-4</v>
       </c>
@@ -9140,7 +8521,7 @@
       <c r="N25" t="s">
         <v>328</v>
       </c>
-      <c r="O25" s="15">
+      <c r="O25" s="14">
         <f>(O19+O21)*O$30+O20*O$31+O22*O$32+O23*O$33+O24*O$29</f>
         <v>3.0494E-2</v>
       </c>
@@ -9173,7 +8554,7 @@
       <c r="N26" t="s">
         <v>330</v>
       </c>
-      <c r="O26" s="15">
+      <c r="O26" s="14">
         <f>O20*O$45+(O23+O24)*O$44</f>
         <v>4.2314285714285709E-3</v>
       </c>
@@ -9206,7 +8587,7 @@
       <c r="N27" t="s">
         <v>340</v>
       </c>
-      <c r="O27" s="15">
+      <c r="O27" s="14">
         <v>3.1300000000000001E-2</v>
       </c>
       <c r="P27" t="s">
@@ -9238,7 +8619,7 @@
       <c r="N28" t="s">
         <v>342</v>
       </c>
-      <c r="O28" s="15">
+      <c r="O28" s="14">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="P28" t="s">
@@ -9270,7 +8651,7 @@
       <c r="N29" t="s">
         <v>344</v>
       </c>
-      <c r="O29" s="15">
+      <c r="O29" s="14">
         <v>0.03</v>
       </c>
       <c r="P29" t="s">
@@ -9302,7 +8683,7 @@
       <c r="N30" t="s">
         <v>346</v>
       </c>
-      <c r="O30" s="15">
+      <c r="O30" s="14">
         <v>3.1300000000000001E-2</v>
       </c>
       <c r="P30" t="s">
@@ -9334,7 +8715,7 @@
       <c r="N31" t="s">
         <v>348</v>
       </c>
-      <c r="O31" s="15">
+      <c r="O31" s="14">
         <v>0.03</v>
       </c>
       <c r="P31" t="s">
@@ -9366,7 +8747,7 @@
       <c r="N32" t="s">
         <v>350</v>
       </c>
-      <c r="O32" s="15">
+      <c r="O32" s="14">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="P32" t="s">
@@ -9398,7 +8779,7 @@
       <c r="N33" t="s">
         <v>352</v>
       </c>
-      <c r="O33" s="15">
+      <c r="O33" s="14">
         <v>0.03</v>
       </c>
       <c r="P33" t="s">
@@ -9427,7 +8808,7 @@
       <c r="N34" t="s">
         <v>354</v>
       </c>
-      <c r="O34" s="15">
+      <c r="O34" s="14">
         <v>3.1300000000000001E-2</v>
       </c>
       <c r="P34" t="s">
@@ -9456,7 +8837,7 @@
       <c r="N35" t="s">
         <v>356</v>
       </c>
-      <c r="O35" s="15">
+      <c r="O35" s="14">
         <v>0.03</v>
       </c>
       <c r="P35" t="s">
@@ -9476,7 +8857,7 @@
       <c r="I36" s="1">
         <v>1E-4</v>
       </c>
-      <c r="O36" s="15"/>
+      <c r="O36" s="14"/>
     </row>
     <row r="37" spans="7:17" x14ac:dyDescent="0.35">
       <c r="G37" t="s">
@@ -9494,7 +8875,7 @@
       <c r="K37" t="s">
         <v>436</v>
       </c>
-      <c r="O37" s="15"/>
+      <c r="O37" s="14"/>
     </row>
     <row r="38" spans="7:17" ht="16.5" x14ac:dyDescent="0.35">
       <c r="G38" t="s">
@@ -9518,7 +8899,7 @@
       <c r="N38" t="s">
         <v>358</v>
       </c>
-      <c r="O38" s="15">
+      <c r="O38" s="14">
         <v>2.1700000000000001E-2</v>
       </c>
       <c r="P38" t="s">
@@ -9547,7 +8928,7 @@
       <c r="N39" t="s">
         <v>360</v>
       </c>
-      <c r="O39" s="15">
+      <c r="O39" s="14">
         <v>2.4E-2</v>
       </c>
       <c r="P39" t="s">
@@ -9576,7 +8957,7 @@
       <c r="N40" t="s">
         <v>362</v>
       </c>
-      <c r="O40" s="15">
+      <c r="O40" s="14">
         <v>2.6800000000000001E-2</v>
       </c>
       <c r="P40" t="s">
@@ -9609,7 +8990,7 @@
       <c r="N41" t="s">
         <v>364</v>
       </c>
-      <c r="O41" s="15">
+      <c r="O41" s="14">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="P41" t="s">
@@ -9626,7 +9007,7 @@
       <c r="N42" t="s">
         <v>366</v>
       </c>
-      <c r="O42" s="15">
+      <c r="O42" s="14">
         <v>3.1300000000000001E-2</v>
       </c>
       <c r="P42" t="s">
@@ -9643,7 +9024,7 @@
       <c r="N43" t="s">
         <v>368</v>
       </c>
-      <c r="O43" s="15">
+      <c r="O43" s="14">
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="P43" t="s">
@@ -9660,7 +9041,7 @@
       <c r="N44" t="s">
         <v>370</v>
       </c>
-      <c r="O44" s="15">
+      <c r="O44" s="14">
         <v>4.2857142857142859E-3</v>
       </c>
       <c r="P44" t="s">
@@ -9677,7 +9058,7 @@
       <c r="N45" t="s">
         <v>356</v>
       </c>
-      <c r="O45" s="15">
+      <c r="O45" s="14">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="P45" t="s">
@@ -9775,7 +9156,7 @@
       <c r="N52" t="s">
         <v>186</v>
       </c>
-      <c r="O52" s="20">
+      <c r="O52" s="9">
         <v>5.5055388903508104E-3</v>
       </c>
       <c r="Q52" t="s">
@@ -9786,7 +9167,7 @@
       <c r="M53" t="s">
         <v>192</v>
       </c>
-      <c r="O53" s="21">
+      <c r="O53">
         <v>0.1744</v>
       </c>
       <c r="P53" t="s">
@@ -9800,7 +9181,7 @@
       <c r="M54" t="s">
         <v>138</v>
       </c>
-      <c r="O54" s="21">
+      <c r="O54">
         <v>0.06</v>
       </c>
       <c r="P54" t="s">
@@ -9814,7 +9195,7 @@
       <c r="M55" t="s">
         <v>60</v>
       </c>
-      <c r="O55" s="21">
+      <c r="O55">
         <v>4.7E-2</v>
       </c>
       <c r="P55" t="s">
@@ -9828,7 +9209,7 @@
       <c r="M56" t="s">
         <v>59</v>
       </c>
-      <c r="O56" s="21">
+      <c r="O56">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="P56" t="s">

</xml_diff>